<commit_message>
Implementing Raw DT, Get Trending and Get Quotes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\OneDrive\Documents\UiPath\AutomatingFinancialDataManagement\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2BE4C9-9BB7-4D4D-8A60-A856BDDD1982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A897E3-B970-4091-9CA7-FAF2738229C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1236" yWindow="624" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>https://query2.finance.yahoo.com/v10/finance/quoteSummary/{ticker}?modules=calendarEvents,price&amp;lang=en-US&amp;region=US&amp;corsDomain=finance.yahoo.com</t>
+  </si>
+  <si>
+    <t>BatchSize</t>
+  </si>
+  <si>
+    <t>DelayBetweenBatchesMs</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -495,7 +501,7 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -520,6 +526,22 @@
       </c>
       <c r="B12" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comment Out - Quote Extraction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\OneDrive\Documents\UiPath\AutomatingFinancialDataManagement\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A897E3-B970-4091-9CA7-FAF2738229C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D67E62-CD59-4DED-A2FE-47A85908BAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1236" yWindow="624" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Logs\run.log</t>
   </si>
   <si>
-    <t>YahooFinanceUrl</t>
-  </si>
-  <si>
     <t>TopMoversThresholdPercent</t>
   </si>
   <si>
@@ -72,25 +69,10 @@
     <t>Data\Output</t>
   </si>
   <si>
-    <t>https://query1.finance.yahoo.com/v1/finance/trending/US?lang=en-US&amp;region=US&amp;count=50&amp;corsDomain=finance.yahoo.com</t>
-  </si>
-  <si>
     <t>TrendingUrlTemplate</t>
   </si>
   <si>
     <t>https://query1.finance.yahoo.com/v1/finance/trending/US?lang=en-US&amp;region=US&amp;count={count}&amp;corsDomain=finance.yahoo.com</t>
-  </si>
-  <si>
-    <t>QuoteUrlTemplate</t>
-  </si>
-  <si>
-    <t>QuoteSummaryUrlTemplate</t>
-  </si>
-  <si>
-    <t>https://query1.finance.yahoo.com/v7/finance/quote?lang=en-US&amp;region=US&amp;corsDomain=finance.yahoo.com&amp;symbols={symbols}</t>
-  </si>
-  <si>
-    <t>https://query2.finance.yahoo.com/v10/finance/quoteSummary/{ticker}?modules=calendarEvents,price&amp;lang=en-US&amp;region=US&amp;corsDomain=finance.yahoo.com</t>
   </si>
   <si>
     <t>BatchSize</t>
@@ -420,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -442,10 +424,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -481,11 +463,11 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
+      <c r="B7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -493,54 +475,30 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>20</v>
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
+      <c r="B10">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
+        <v>17</v>
+      </c>
+      <c r="B11">
         <v>700</v>
       </c>
     </row>

</xml_diff>